<commit_message>
agregue una hoja al archivo excel
</commit_message>
<xml_diff>
--- a/TCM.xlsx
+++ b/TCM.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>A</t>
   </si>
@@ -61,6 +62,15 @@
   </si>
   <si>
     <t>V(T)=A*c</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>h(i)=h(i-1)+(E(i)-S(i))*∆t/A</t>
+  </si>
+  <si>
+    <t>K*T</t>
   </si>
 </sst>
 </file>
@@ -70,7 +80,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -89,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -168,8 +184,33 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A4" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +849,7 @@
         <f t="shared" si="2"/>
         <v>19.200000000000003</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="17">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -817,4 +858,580 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="20">
+        <v>2</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
+        <f>$E$1</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>$E$2*B6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <f>B2</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="22">
+        <f>$E$3</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="23">
+        <f>$B$1*E6</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B6+$B$3</f>
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" ref="C7:C22" si="0">$E$1</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D22" si="1">$E$2*B7</f>
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="22">
+        <f>E6+(C7-D7)*$B$3/$B$1</f>
+        <v>4.96</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" ref="F7:F22" si="2">$E$3</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" ref="G7:G22" si="3">$B$1*E7</f>
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B7+$B$3</f>
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" ref="E8:E22" si="4">E7+(C8-D8)*$B$3/$B$1</f>
+        <v>4.88</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="3"/>
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" ref="B9:B22" si="5">B8+$B$3</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="4"/>
+        <v>4.76</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="3"/>
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" si="4"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F10" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="3"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="4"/>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="F11" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="3"/>
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="4"/>
+        <v>4.1599999999999993</v>
+      </c>
+      <c r="F12" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="3"/>
+        <v>2.0799999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="E13" s="22">
+        <f t="shared" si="4"/>
+        <v>3.8799999999999994</v>
+      </c>
+      <c r="F13" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="3"/>
+        <v>1.9399999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="5"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="E14" s="22">
+        <f t="shared" si="4"/>
+        <v>3.5599999999999996</v>
+      </c>
+      <c r="F14" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="3"/>
+        <v>1.7799999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="5"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E15" s="22">
+        <f t="shared" si="4"/>
+        <v>3.1999999999999997</v>
+      </c>
+      <c r="F15" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="3"/>
+        <v>1.5999999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="E16" s="22">
+        <f t="shared" si="4"/>
+        <v>2.8</v>
+      </c>
+      <c r="F16" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="3"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="E17" s="22">
+        <f t="shared" si="4"/>
+        <v>2.36</v>
+      </c>
+      <c r="F17" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="3"/>
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" si="4"/>
+        <v>1.88</v>
+      </c>
+      <c r="F18" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="3"/>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="5"/>
+        <v>1.3</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" si="4"/>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="F19" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="3"/>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="5"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="E20" s="22">
+        <f t="shared" si="4"/>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="F20" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G20" s="23">
+        <f t="shared" si="3"/>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="5"/>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="E21" s="22">
+        <f t="shared" si="4"/>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="F21" s="22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G21" s="23">
+        <f t="shared" si="3"/>
+        <v>9.9999999999999867E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>16</v>
+      </c>
+      <c r="B22" s="6">
+        <f t="shared" si="5"/>
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000006</v>
+      </c>
+      <c r="E22" s="24">
+        <f t="shared" si="4"/>
+        <v>-0.44000000000000039</v>
+      </c>
+      <c r="F22" s="24">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G22" s="25">
+        <f t="shared" si="3"/>
+        <v>-0.2200000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregue hojas al archivo excel
</commit_message>
<xml_diff>
--- a/TCM.xlsx
+++ b/TCM.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>A</t>
   </si>
@@ -71,18 +73,34 @@
   </si>
   <si>
     <t>K*T</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>w*t^2</t>
+  </si>
+  <si>
+    <t>h(i ) = h(i-1) + (E(i ) - S(i )) * Δt  / A</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>g/a*h(t)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +115,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -158,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +235,27 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1434,4 +1480,484 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>12</v>
+      </c>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
+        <f>$E$1</f>
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <f>$E$2*(B6^2)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <f>$E$3</f>
+        <v>8</v>
+      </c>
+      <c r="G6" s="15">
+        <f>$B$1*E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B6+$B$3</f>
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" ref="C7:C10" si="0">$E$1</f>
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <f>$E$2*(B7^2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="22">
+        <f>E6+(C7-D7)*$B$3/$B$1</f>
+        <v>2.875</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" ref="F7:F10" si="1">$E$3</f>
+        <v>8</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" ref="G7:G10" si="2">$B$1*E7</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <f t="shared" ref="B8:B10" si="3">B7+$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" ref="D8:D10" si="4">$E$2*(B8^2)</f>
+        <v>2</v>
+      </c>
+      <c r="E8" s="29">
+        <f t="shared" ref="E8:E10" si="5">E7+(C8-D8)*$B$3/$B$1</f>
+        <v>5.375</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="2"/>
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="5"/>
+        <v>7.25</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="5"/>
+        <v>8.25</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="2"/>
+        <v>16.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>1</v>
+      </c>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
+        <f>$E$1</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f>$E$2*B2</f>
+        <v>0.125</v>
+      </c>
+      <c r="E6" s="30">
+        <f>B2</f>
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="22">
+        <f>$E$3</f>
+        <v>3.75</v>
+      </c>
+      <c r="G6" s="15">
+        <f>$B$1*E6</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <f>B6+$B$3</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" ref="C7:C10" si="0">$E$1</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <f>$E$2*E6</f>
+        <v>0.125</v>
+      </c>
+      <c r="E7" s="31">
+        <f>E6+(C7-D7)*$B$3/$B$1</f>
+        <v>2.25</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" ref="F7:F10" si="1">$E$3</f>
+        <v>3.75</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" ref="G7:G10" si="2">$B$1*E7</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" ref="B8:B10" si="3">B7+$B$3</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:D10" si="4">$E$2*E7</f>
+        <v>0.5625</v>
+      </c>
+      <c r="E8" s="30">
+        <f t="shared" ref="E8:E10" si="5">E7+(C8-D8)*$B$3/$B$1</f>
+        <v>3.125</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="2"/>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="4"/>
+        <v>0.78125</v>
+      </c>
+      <c r="E9" s="30">
+        <f t="shared" si="5"/>
+        <v>3.5625</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="2"/>
+        <v>3.5625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="4"/>
+        <v>0.890625</v>
+      </c>
+      <c r="E10" s="32">
+        <f t="shared" si="5"/>
+        <v>3.78125</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="2"/>
+        <v>3.78125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modifique una celda del archivo
</commit_message>
<xml_diff>
--- a/TCM.xlsx
+++ b/TCM.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1486,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1521,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>18</v>
@@ -1615,11 +1616,11 @@
       </c>
       <c r="D7" s="1">
         <f>$E$2*(B7^2)</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E7" s="22">
         <f>E6+(C7-D7)*$B$3/$B$1</f>
-        <v>2.875</v>
+        <v>2.8125</v>
       </c>
       <c r="F7" s="22">
         <f t="shared" ref="F7:F10" si="1">$E$3</f>
@@ -1627,7 +1628,7 @@
       </c>
       <c r="G7" s="15">
         <f t="shared" ref="G7:G10" si="2">$B$1*E7</f>
-        <v>5.75</v>
+        <v>5.625</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1644,11 +1645,11 @@
       </c>
       <c r="D8" s="7">
         <f t="shared" ref="D8:D10" si="4">$E$2*(B8^2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="29">
         <f t="shared" ref="E8:E10" si="5">E7+(C8-D8)*$B$3/$B$1</f>
-        <v>5.375</v>
+        <v>5.0625</v>
       </c>
       <c r="F8" s="22">
         <f t="shared" si="1"/>
@@ -1656,7 +1657,7 @@
       </c>
       <c r="G8" s="15">
         <f t="shared" si="2"/>
-        <v>10.75</v>
+        <v>10.125</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,11 +1674,11 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>6.75</v>
       </c>
       <c r="E9" s="22">
         <f t="shared" si="5"/>
-        <v>7.25</v>
+        <v>6.375</v>
       </c>
       <c r="F9" s="22">
         <f t="shared" si="1"/>
@@ -1685,7 +1686,7 @@
       </c>
       <c r="G9" s="15">
         <f t="shared" si="2"/>
-        <v>14.5</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,19 +1703,19 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="5"/>
+        <v>6.375</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E10" s="24">
-        <f t="shared" si="5"/>
-        <v>8.25</v>
-      </c>
-      <c r="F10" s="24">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
       <c r="G10" s="16">
         <f t="shared" si="2"/>
-        <v>16.5</v>
+        <v>12.75</v>
       </c>
     </row>
   </sheetData>
@@ -1726,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,4 +1961,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>